<commit_message>
debug club name matching in round participation calc
</commit_message>
<xml_diff>
--- a/data/processed/Sydney League 1 Round 1 IRONMAN 70.3 and Sprint ACTUAL.xlsx
+++ b/data/processed/Sydney League 1 Round 1 IRONMAN 70.3 and Sprint ACTUAL.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,12 +423,9 @@
         <v xml:space="preserve">Category Finish Place </v>
       </c>
       <c r="F1" t="str">
-        <v>Manual Calcs</v>
+        <v xml:space="preserve">Club Name </v>
       </c>
       <c r="G1" t="str">
-        <v xml:space="preserve">Club Name </v>
-      </c>
-      <c r="H1" t="str">
         <v>Performance points Participation points or both</v>
       </c>
     </row>
@@ -449,12 +446,9 @@
         <v>27</v>
       </c>
       <c r="F2" t="str">
-        <v>0</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G2" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H2" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -475,12 +469,9 @@
         <v>57</v>
       </c>
       <c r="F3" t="str">
-        <v>0</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G3" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H3" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -501,12 +492,9 @@
         <v>59</v>
       </c>
       <c r="F4" t="str">
-        <v>0</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G4" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H4" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -527,12 +515,9 @@
         <v>17</v>
       </c>
       <c r="F5" t="str">
-        <v>0</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G5" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H5" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -553,12 +538,9 @@
         <v>15</v>
       </c>
       <c r="F6" t="str">
-        <v>0</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G6" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H6" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -579,12 +561,9 @@
         <v>22</v>
       </c>
       <c r="F7" t="str">
-        <v>0</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G7" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H7" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -605,12 +584,9 @@
         <v>20</v>
       </c>
       <c r="F8" t="str">
-        <v>0</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G8" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H8" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -631,12 +607,9 @@
         <v>3</v>
       </c>
       <c r="F9" t="str">
-        <v>8</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G9" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H9" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -657,12 +630,9 @@
         <v>46</v>
       </c>
       <c r="F10" t="str">
-        <v>0</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G10" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H10" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -683,12 +653,9 @@
         <v>105</v>
       </c>
       <c r="F11" t="str">
-        <v>0</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G11" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H11" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -709,12 +676,9 @@
         <v>13</v>
       </c>
       <c r="F12" t="str">
-        <v>0</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G12" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H12" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -735,12 +699,9 @@
         <v>31</v>
       </c>
       <c r="F13" t="str">
-        <v>0</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G13" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H13" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -761,12 +722,9 @@
         <v>35</v>
       </c>
       <c r="F14" t="str">
-        <v>0</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G14" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H14" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -787,12 +745,9 @@
         <v>48</v>
       </c>
       <c r="F15" t="str">
-        <v>0</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G15" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H15" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -813,12 +768,9 @@
         <v>10</v>
       </c>
       <c r="F16" t="str">
-        <v>1</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G16" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H16" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -839,12 +791,9 @@
         <v>36</v>
       </c>
       <c r="F17" t="str">
-        <v>0</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G17" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H17" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -865,12 +814,9 @@
         <v>1</v>
       </c>
       <c r="F18" t="str">
-        <v>10</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G18" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H18" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -891,12 +837,9 @@
         <v>13</v>
       </c>
       <c r="F19" t="str">
-        <v>0</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G19" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H19" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -917,12 +860,9 @@
         <v>3</v>
       </c>
       <c r="F20" t="str">
-        <v>8</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G20" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H20" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -943,12 +883,9 @@
         <v>43</v>
       </c>
       <c r="F21" t="str">
-        <v>0</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G21" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H21" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -969,12 +906,9 @@
         <v>72</v>
       </c>
       <c r="F22" t="str">
-        <v>0</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G22" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H22" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -995,12 +929,9 @@
         <v>96</v>
       </c>
       <c r="F23" t="str">
-        <v>0</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G23" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H23" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1021,12 +952,9 @@
         <v>161</v>
       </c>
       <c r="F24" t="str">
-        <v>0</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G24" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H24" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1047,12 +975,9 @@
         <v>87</v>
       </c>
       <c r="F25" t="str">
-        <v>0</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G25" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H25" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1073,12 +998,9 @@
         <v>24</v>
       </c>
       <c r="F26" t="str">
-        <v>0</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G26" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H26" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1099,12 +1021,9 @@
         <v>10</v>
       </c>
       <c r="F27" t="str">
-        <v>1</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G27" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H27" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1125,12 +1044,9 @@
         <v>9</v>
       </c>
       <c r="F28" t="str">
-        <v>2</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G28" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H28" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1151,12 +1067,9 @@
         <v>13</v>
       </c>
       <c r="F29" t="str">
-        <v>0</v>
+        <v>Engadine Triathlon Club</v>
       </c>
       <c r="G29" t="str">
-        <v>Engadine Triathlon Club</v>
-      </c>
-      <c r="H29" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1177,12 +1090,9 @@
         <v>24</v>
       </c>
       <c r="F30" t="str">
-        <v>0</v>
+        <v>Engadine Triathlon Club</v>
       </c>
       <c r="G30" t="str">
-        <v>Engadine Triathlon Club</v>
-      </c>
-      <c r="H30" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1203,12 +1113,9 @@
         <v>68</v>
       </c>
       <c r="F31" t="str">
-        <v>0</v>
+        <v>FILOZ TRIATHLON CLUB</v>
       </c>
       <c r="G31" t="str">
-        <v>FILOZ TRIATHLON CLUB</v>
-      </c>
-      <c r="H31" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1229,12 +1136,9 @@
         <v>2</v>
       </c>
       <c r="F32" t="str">
-        <v>9</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G32" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H32" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1255,12 +1159,9 @@
         <v>34</v>
       </c>
       <c r="F33" t="str">
-        <v>0</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G33" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H33" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1281,12 +1182,9 @@
         <v>12</v>
       </c>
       <c r="F34" t="str">
-        <v>0</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G34" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H34" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1307,12 +1205,9 @@
         <v>76</v>
       </c>
       <c r="F35" t="str">
-        <v>0</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G35" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H35" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1333,12 +1228,9 @@
         <v>6</v>
       </c>
       <c r="F36" t="str">
-        <v>5</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G36" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H36" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1359,12 +1251,9 @@
         <v>234</v>
       </c>
       <c r="F37" t="str">
-        <v>0</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G37" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H37" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1385,12 +1274,9 @@
         <v>39</v>
       </c>
       <c r="F38" t="str">
-        <v>0</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G38" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H38" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1411,12 +1297,9 @@
         <v>56</v>
       </c>
       <c r="F39" t="str">
-        <v>0</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G39" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H39" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1437,12 +1320,9 @@
         <v>62</v>
       </c>
       <c r="F40" t="str">
-        <v>0</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G40" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H40" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1463,12 +1343,9 @@
         <v>85</v>
       </c>
       <c r="F41" t="str">
-        <v>0</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G41" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H41" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1489,12 +1366,9 @@
         <v>3</v>
       </c>
       <c r="F42" t="str">
-        <v>8</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G42" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H42" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1515,12 +1389,9 @@
         <v>38</v>
       </c>
       <c r="F43" t="str">
-        <v>0</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G43" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H43" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1541,12 +1412,9 @@
         <v>8</v>
       </c>
       <c r="F44" t="str">
-        <v>3</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G44" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H44" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1567,12 +1435,9 @@
         <v>19</v>
       </c>
       <c r="F45" t="str">
-        <v>0</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G45" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H45" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1593,12 +1458,9 @@
         <v>5</v>
       </c>
       <c r="F46" t="str">
-        <v>6</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G46" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H46" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1619,12 +1481,9 @@
         <v>1</v>
       </c>
       <c r="F47" t="str">
-        <v>10</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G47" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H47" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1645,12 +1504,9 @@
         <v>9</v>
       </c>
       <c r="F48" t="str">
-        <v>2</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G48" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H48" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1671,12 +1527,9 @@
         <v>2</v>
       </c>
       <c r="F49" t="str">
-        <v>9</v>
+        <v>Moore Performance Triathlon Club</v>
       </c>
       <c r="G49" t="str">
-        <v>Moore Performance Triathlon Club</v>
-      </c>
-      <c r="H49" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1697,12 +1550,9 @@
         <v>41</v>
       </c>
       <c r="F50" t="str">
-        <v>0</v>
+        <v>Moore Performance Triathlon Club</v>
       </c>
       <c r="G50" t="str">
-        <v>Moore Performance Triathlon Club</v>
-      </c>
-      <c r="H50" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1723,12 +1573,9 @@
         <v>7</v>
       </c>
       <c r="F51" t="str">
-        <v>4</v>
+        <v>Moore Performance Triathlon Club</v>
       </c>
       <c r="G51" t="str">
-        <v>Moore Performance Triathlon Club</v>
-      </c>
-      <c r="H51" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1749,12 +1596,9 @@
         <v>17</v>
       </c>
       <c r="F52" t="str">
-        <v>0</v>
+        <v>Moore Performance Triathlon Club</v>
       </c>
       <c r="G52" t="str">
-        <v>Moore Performance Triathlon Club</v>
-      </c>
-      <c r="H52" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1775,12 +1619,9 @@
         <v>4</v>
       </c>
       <c r="F53" t="str">
-        <v>7</v>
+        <v>Moore Performance Triathlon Club</v>
       </c>
       <c r="G53" t="str">
-        <v>Moore Performance Triathlon Club</v>
-      </c>
-      <c r="H53" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1801,12 +1642,9 @@
         <v>2</v>
       </c>
       <c r="F54" t="str">
-        <v>9</v>
+        <v>Moore Performance Triathlon Club</v>
       </c>
       <c r="G54" t="str">
-        <v>Moore Performance Triathlon Club</v>
-      </c>
-      <c r="H54" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1827,12 +1665,9 @@
         <v>172</v>
       </c>
       <c r="F55" t="str">
-        <v>0</v>
+        <v>Moore Performance Triathlon Club</v>
       </c>
       <c r="G55" t="str">
-        <v>Moore Performance Triathlon Club</v>
-      </c>
-      <c r="H55" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1853,12 +1688,9 @@
         <v>30</v>
       </c>
       <c r="F56" t="str">
-        <v>0</v>
+        <v>Northern Suburbs Triathlon Club</v>
       </c>
       <c r="G56" t="str">
-        <v>Northern Suburbs Triathlon Club</v>
-      </c>
-      <c r="H56" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1879,12 +1711,9 @@
         <v>6</v>
       </c>
       <c r="F57" t="str">
-        <v>5</v>
+        <v>Northern Suburbs Triathlon Club</v>
       </c>
       <c r="G57" t="str">
-        <v>Northern Suburbs Triathlon Club</v>
-      </c>
-      <c r="H57" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1905,12 +1734,9 @@
         <v>7</v>
       </c>
       <c r="F58" t="str">
-        <v>4</v>
+        <v>Northern Suburbs Triathlon Club</v>
       </c>
       <c r="G58" t="str">
-        <v>Northern Suburbs Triathlon Club</v>
-      </c>
-      <c r="H58" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1931,12 +1757,9 @@
         <v>20</v>
       </c>
       <c r="F59" t="str">
-        <v>0</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G59" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H59" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1957,12 +1780,9 @@
         <v>1</v>
       </c>
       <c r="F60" t="str">
-        <v>10</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G60" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H60" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -1983,12 +1803,9 @@
         <v>37</v>
       </c>
       <c r="F61" t="str">
-        <v>0</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G61" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H61" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2009,12 +1826,9 @@
         <v>56</v>
       </c>
       <c r="F62" t="str">
-        <v>0</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G62" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H62" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2035,12 +1849,9 @@
         <v>5</v>
       </c>
       <c r="F63" t="str">
-        <v>6</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G63" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H63" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2061,12 +1872,9 @@
         <v>71</v>
       </c>
       <c r="F64" t="str">
-        <v>0</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G64" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H64" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2087,12 +1895,9 @@
         <v>12</v>
       </c>
       <c r="F65" t="str">
-        <v>0</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G65" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H65" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2113,12 +1918,9 @@
         <v>14</v>
       </c>
       <c r="F66" t="str">
-        <v>0</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G66" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H66" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2139,12 +1941,9 @@
         <v>63</v>
       </c>
       <c r="F67" t="str">
-        <v>0</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G67" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H67" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2165,12 +1964,9 @@
         <v>1</v>
       </c>
       <c r="F68" t="str">
-        <v>10</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G68" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H68" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2191,12 +1987,9 @@
         <v>11</v>
       </c>
       <c r="F69" t="str">
-        <v>0</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G69" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H69" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2217,12 +2010,9 @@
         <v>39</v>
       </c>
       <c r="F70" t="str">
-        <v>0</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G70" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H70" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2243,12 +2033,9 @@
         <v>54</v>
       </c>
       <c r="F71" t="str">
-        <v>0</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G71" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H71" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2269,12 +2056,9 @@
         <v>73</v>
       </c>
       <c r="F72" t="str">
-        <v>0</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G72" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H72" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2295,12 +2079,9 @@
         <v>9</v>
       </c>
       <c r="F73" t="str">
-        <v>2</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G73" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H73" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2321,12 +2102,9 @@
         <v>2</v>
       </c>
       <c r="F74" t="str">
-        <v>9</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G74" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H74" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2347,25 +2125,22 @@
         <v>24</v>
       </c>
       <c r="F75" t="str">
-        <v>0</v>
+        <v>TriMob</v>
       </c>
       <c r="G75" t="str">
-        <v>TriMob</v>
-      </c>
-      <c r="H75" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H75"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G75"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2387,12 +2162,9 @@
         <v xml:space="preserve">Category Finish Place </v>
       </c>
       <c r="F1" t="str">
-        <v>Manual Calcs</v>
+        <v xml:space="preserve">Club Name </v>
       </c>
       <c r="G1" t="str">
-        <v xml:space="preserve">Club Name </v>
-      </c>
-      <c r="H1" t="str">
         <v>Performance points Participation points or both</v>
       </c>
     </row>
@@ -2413,12 +2185,9 @@
         <v>12</v>
       </c>
       <c r="F2" t="str">
-        <v>0</v>
+        <v>BRAT Triathlon Club</v>
       </c>
       <c r="G2" t="str">
-        <v>BRAT Triathlon Club</v>
-      </c>
-      <c r="H2" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2439,12 +2208,9 @@
         <v>6</v>
       </c>
       <c r="F3" t="str">
-        <v>5</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G3" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H3" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2465,12 +2231,9 @@
         <v>1</v>
       </c>
       <c r="F4" t="str">
-        <v>10</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G4" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H4" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2491,12 +2254,9 @@
         <v>8</v>
       </c>
       <c r="F5" t="str">
-        <v>3</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G5" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H5" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2517,12 +2277,9 @@
         <v>18</v>
       </c>
       <c r="F6" t="str">
-        <v>0</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G6" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H6" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2543,12 +2300,9 @@
         <v>10</v>
       </c>
       <c r="F7" t="str">
-        <v>1</v>
+        <v>Coogee Triathlon Club</v>
       </c>
       <c r="G7" t="str">
-        <v>Coogee Triathlon Club</v>
-      </c>
-      <c r="H7" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2569,12 +2323,9 @@
         <v>22</v>
       </c>
       <c r="F8" t="str">
-        <v>0</v>
+        <v>Engadine Triathlon Club Inc</v>
       </c>
       <c r="G8" t="str">
-        <v>Engadine Triathlon Club Inc</v>
-      </c>
-      <c r="H8" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2595,12 +2346,9 @@
         <v>15</v>
       </c>
       <c r="F9" t="str">
-        <v>0</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G9" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H9" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2621,12 +2369,9 @@
         <v>4</v>
       </c>
       <c r="F10" t="str">
-        <v>7</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G10" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H10" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2647,12 +2392,9 @@
         <v>7</v>
       </c>
       <c r="F11" t="str">
-        <v>4</v>
+        <v>Hills Triathlon Club</v>
       </c>
       <c r="G11" t="str">
-        <v>Hills Triathlon Club</v>
-      </c>
-      <c r="H11" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2673,12 +2415,9 @@
         <v>2</v>
       </c>
       <c r="F12" t="str">
-        <v>9</v>
+        <v>Moore Performance Triathlon Club</v>
       </c>
       <c r="G12" t="str">
-        <v>Moore Performance Triathlon Club</v>
-      </c>
-      <c r="H12" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2699,12 +2438,9 @@
         <v>4</v>
       </c>
       <c r="F13" t="str">
-        <v>7</v>
+        <v>Moore Performance Triathlon Club</v>
       </c>
       <c r="G13" t="str">
-        <v>Moore Performance Triathlon Club</v>
-      </c>
-      <c r="H13" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2725,12 +2461,9 @@
         <v>4</v>
       </c>
       <c r="F14" t="str">
-        <v>7</v>
+        <v>Moore Performance Triathlon Club</v>
       </c>
       <c r="G14" t="str">
-        <v>Moore Performance Triathlon Club</v>
-      </c>
-      <c r="H14" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2751,12 +2484,9 @@
         <v>9</v>
       </c>
       <c r="F15" t="str">
-        <v>2</v>
+        <v>Moore Performance Triathlon Club</v>
       </c>
       <c r="G15" t="str">
-        <v>Moore Performance Triathlon Club</v>
-      </c>
-      <c r="H15" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2777,12 +2507,9 @@
         <v>25</v>
       </c>
       <c r="F16" t="str">
-        <v>0</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G16" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H16" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2803,12 +2530,9 @@
         <v>1</v>
       </c>
       <c r="F17" t="str">
-        <v>10</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G17" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H17" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2829,12 +2553,9 @@
         <v>1</v>
       </c>
       <c r="F18" t="str">
-        <v>10</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G18" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H18" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2855,12 +2576,9 @@
         <v>5</v>
       </c>
       <c r="F19" t="str">
-        <v>6</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G19" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H19" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2881,12 +2599,9 @@
         <v>1</v>
       </c>
       <c r="F20" t="str">
-        <v>10</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G20" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H20" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2907,12 +2622,9 @@
         <v>5</v>
       </c>
       <c r="F21" t="str">
-        <v>6</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G21" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H21" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2933,12 +2645,9 @@
         <v>20</v>
       </c>
       <c r="F22" t="str">
-        <v>0</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G22" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H22" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2959,12 +2668,9 @@
         <v>17</v>
       </c>
       <c r="F23" t="str">
-        <v>0</v>
+        <v>Panthers Triathlon Club</v>
       </c>
       <c r="G23" t="str">
-        <v>Panthers Triathlon Club</v>
-      </c>
-      <c r="H23" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
@@ -2985,18 +2691,15 @@
         <v>12</v>
       </c>
       <c r="F24" t="str">
-        <v>0</v>
+        <v>South West Sydney Triathlon Club</v>
       </c>
       <c r="G24" t="str">
-        <v>Sydney South West Triathlon Club</v>
-      </c>
-      <c r="H24" t="str">
         <v xml:space="preserve">Per P &amp; Part P </v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H24"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G24"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>